<commit_message>
Training after data fixes
</commit_message>
<xml_diff>
--- a/data/zweryfikowane.xlsx
+++ b/data/zweryfikowane.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocalAdmin\document-classification\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F91B058-479D-4EAA-9277-1ACBE6823582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16392"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -26,8 +32,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="modified_dataset" type="6" refreshedVersion="3" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="modified_dataset" type="6" refreshedVersion="3" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="D:\moje foldery\studia\magisterka\semestr 2\Podstawy_Uczenia_Glebokiego\document-classification\data\modified_dataset.csv" decimal="," thousands=" " tab="0" comma="1">
       <textFields count="7">
         <textField/>
@@ -8083,13 +8089,13 @@
     <t>Wartości</t>
   </si>
   <si>
-    <t>czy git</t>
+    <t>quality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -8154,7 +8160,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Wiktorcio" refreshedDate="45263.465136689818" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="2722">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Wiktorcio" refreshedDate="45263.465136689818" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="2722" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B1:B1048576" sheet="Arkusz1"/>
   </cacheSource>
@@ -8208,7 +8214,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Wiktorcio" refreshedDate="45263.465528703702" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="2722">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Wiktorcio" refreshedDate="45263.465528703702" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="2722" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="C1:C1048576" sheet="Arkusz1"/>
   </cacheSource>
@@ -8239,7 +8245,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Wiktorcio" refreshedDate="45263.469666666664" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="2722">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Wiktorcio" refreshedDate="45263.469666666664" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="2722" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B1:C1048576" sheet="Arkusz1"/>
   </cacheSource>
@@ -35544,7 +35550,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="Tabela przestawna1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A3:B39" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0" sortType="descending" countASubtotal="1">
@@ -35726,7 +35732,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="Tabela przestawna2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0" sortType="descending">
@@ -35816,7 +35822,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="Tabela przestawna3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -36052,13 +36058,13 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="modified_dataset" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="modified_dataset" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Pakiet Office 2007–2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -36096,7 +36102,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Pakiet Office 2007–2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -36130,6 +36136,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -36164,9 +36171,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Pakiet Office 2007–2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -36339,23 +36347,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2722"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F7" sqref="F7"/>
+      <selection pane="topRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.5" customWidth="1"/>
-    <col min="2" max="2" width="18.19921875" customWidth="1"/>
-    <col min="3" max="3" width="23.69921875" customWidth="1"/>
-    <col min="4" max="4" width="80.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.25" customWidth="1"/>
+    <col min="3" max="3" width="23.75" customWidth="1"/>
+    <col min="4" max="4" width="80.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
         <v>2679</v>
       </c>
@@ -74452,9 +74460,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D2722">
-    <filterColumn colId="2"/>
-    <sortState ref="A2:D2722">
+  <autoFilter ref="A1:D2722" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D2722">
       <sortCondition ref="D1:D2722"/>
     </sortState>
   </autoFilter>
@@ -74464,19 +74471,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" customWidth="1"/>
-    <col min="3" max="35" width="52.09765625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="3" max="35" width="52.125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2">
@@ -74778,17 +74785,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2">
@@ -74906,18 +74913,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:C52"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="50.69921875" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.75" customWidth="1"/>
+    <col min="2" max="2" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">

</xml_diff>